<commit_message>
added a couple of review comments
</commit_message>
<xml_diff>
--- a/Documents/ReviewComments.xlsx
+++ b/Documents/ReviewComments.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hbolak01c\Desktop\Documents\BSA Projects\Century\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Century\Century_old_testng\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>S.No</t>
   </si>
@@ -111,6 +114,26 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I observe that we have not implemented the isValidPage method (abstract method from Page.java) in all our page classes. We should implement this for every page to look for an element on that page to identify that it is in the same page
+ @Override
+ protected boolean isValidPage() {
+  return false;
+ }
+</t>
+  </si>
+  <si>
+    <t>src/test/java/com/comcast/century/cm/pages
+src/test/java/com/comcast/century/cm/pages</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>We should use the id/class locator instead of xpath when we are referencing the id/class property in the xpath string.
+For e.g. in the below webelements, we should change the findby attribute to id instead of xpath
+@FindBy(xpath = "//*[@id='addcontact-toolEl']")</t>
   </si>
 </sst>
 </file>
@@ -199,8 +222,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -475,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,9 +724,57 @@
         <v>42622</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="5">
+        <v>42640</v>
+      </c>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="5">
+        <v>42640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Review tracker
</commit_message>
<xml_diff>
--- a/Documents/ReviewComments.xlsx
+++ b/Documents/ReviewComments.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\Century\Century_old_testng\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14040" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,8 @@
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>S.No</t>
   </si>
@@ -158,6 +154,15 @@
   </si>
   <si>
     <t>Rijin/Kesavan/Jatin/Kalyan</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Kesavan</t>
   </si>
 </sst>
 </file>
@@ -193,7 +198,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +208,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,19 +230,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +243,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -550,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,191 +584,210 @@
     <col min="4" max="4" width="44.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="45" style="1"/>
+    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="45" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:11" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="7">
         <v>42615</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="8">
         <v>42622</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:11" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="7">
         <v>42615</v>
       </c>
-      <c r="I3" s="6">
+      <c r="J3" s="8">
         <v>42622</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="91.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:11" s="5" customFormat="1" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="7">
         <v>42615</v>
       </c>
-      <c r="I4" s="6">
+      <c r="J4" s="8">
         <v>42622</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:11" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="7">
         <v>42615</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="8">
         <v>42622</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="7">
         <v>42615</v>
       </c>
-      <c r="I6" s="6">
+      <c r="J6" s="8">
         <v>42622</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -767,41 +806,47 @@
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="2">
         <v>42640</v>
       </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" s="5" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="5">
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="7">
         <v>42640</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="J8" s="8">
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -820,14 +865,14 @@
       <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="2">
         <v>42643</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -846,14 +891,14 @@
       <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="2">
         <v>42646</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -872,40 +917,46 @@
       <c r="F11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="2">
         <v>42646</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="12" spans="1:11" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="7">
         <v>42646</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="J12" s="8">
+        <v>42647</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -924,10 +975,10 @@
       <c r="F13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="2">
         <v>42646</v>
       </c>
     </row>

</xml_diff>